<commit_message>
change in column name
</commit_message>
<xml_diff>
--- a/web/uploads/round5/survey.xlsx
+++ b/web/uploads/round5/survey.xlsx
@@ -1470,12 +1470,6 @@
     <t>Caste ethnicity</t>
   </si>
   <si>
-    <t xml:space="preserve">If  other  what is your caste </t>
-  </si>
-  <si>
-    <t>If other occupa</t>
-  </si>
-  <si>
     <t>Do you have any health problem</t>
   </si>
   <si>
@@ -1576,6 +1570,12 @@
   </si>
   <si>
     <t xml:space="preserve"> 8a If other who has this increased risk come from?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other  caste </t>
+  </si>
+  <si>
+    <t>Other occupation</t>
   </si>
 </sst>
 </file>
@@ -1813,9 +1813,9 @@
     <tableColumn id="20" name="Age"/>
     <tableColumn id="21" name="Gender"/>
     <tableColumn id="22" name="Caste ethnicity"/>
-    <tableColumn id="23" name="If  other  what is your caste "/>
+    <tableColumn id="23" name="Other  caste "/>
     <tableColumn id="24" name="Occupation"/>
-    <tableColumn id="25" name="If other occupa"/>
+    <tableColumn id="25" name="Other occupation"/>
     <tableColumn id="26" name="Do you have any health problem"/>
     <tableColumn id="28" name=" 1 Are your main problems being addressed?"/>
     <tableColumn id="29" name=" 1a What is your biggest problem?"/>
@@ -2143,7 +2143,7 @@
   <dimension ref="A1:AS1401"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2225,115 +2225,115 @@
         <v>482</v>
       </c>
       <c r="I1" t="s">
-        <v>483</v>
+        <v>517</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
       </c>
       <c r="K1" t="s">
+        <v>518</v>
+      </c>
+      <c r="L1" t="s">
+        <v>483</v>
+      </c>
+      <c r="M1" t="s">
         <v>484</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>485</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>486</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>487</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>488</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>489</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>490</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>491</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>492</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>493</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>494</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>495</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>496</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>497</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>498</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>499</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>500</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>501</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>502</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>503</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>504</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>505</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>506</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>507</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>508</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>509</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>510</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>511</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>512</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>513</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>514</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>515</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>516</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>517</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="2" spans="1:45">

</xml_diff>